<commit_message>
Finished categorical variable pre processing
</commit_message>
<xml_diff>
--- a/dummy_variables_tracker.xlsx
+++ b/dummy_variables_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b511a50edbd69fea/Documentos OD/Old One Drive/Documentos/Github Proyects/Lending-Club-Credit-RIsk-Model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="8_{7B3DDDCE-1034-459F-88FF-F4F9DD054507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE226547-698E-4984-B412-DDC1CD435E55}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="8_{7B3DDDCE-1034-459F-88FF-F4F9DD054507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D00CA5E6-51BA-475D-883E-A0D92BA011EF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6CA0EF98-DB53-4FB4-885C-53E294792A95}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Original variable</t>
   </si>
@@ -114,6 +114,27 @@
   </si>
   <si>
     <t>addr_state:WV_NH_WY_DC_ME_ID</t>
+  </si>
+  <si>
+    <t>addr_state:NY</t>
+  </si>
+  <si>
+    <t>addr_state:CA</t>
+  </si>
+  <si>
+    <t>addr_state:IL_TX</t>
+  </si>
+  <si>
+    <t>verification_status</t>
+  </si>
+  <si>
+    <t>verification_status:Verified</t>
+  </si>
+  <si>
+    <t>verification_status:Source Verified</t>
+  </si>
+  <si>
+    <t>verification_status:Not Verified</t>
   </si>
 </sst>
 </file>
@@ -569,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FD8EA91-57EC-41A2-A2B0-E4E6E38EFC0C}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -581,7 +602,8 @@
     <col min="2" max="2" width="11.5546875" style="7"/>
     <col min="3" max="3" width="37.77734375" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.21875" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="11.5546875" style="7"/>
+    <col min="5" max="5" width="29.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.5546875" style="7"/>
     <col min="8" max="16384" width="11.5546875" style="8"/>
   </cols>
   <sheetData>
@@ -598,7 +620,9 @@
       <c r="D1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
@@ -615,7 +639,9 @@
       <c r="D2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
@@ -632,13 +658,19 @@
       <c r="D3" s="10" t="s">
         <v>16</v>
       </c>
+      <c r="E3" s="7" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>17</v>
+        <v>26</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -646,7 +678,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -654,7 +686,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -662,7 +694,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -670,26 +702,41 @@
         <v>10</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D9" s="10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D10" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D11" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D12" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D13" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D14" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D15" s="10" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>